<commit_message>
14.5. - pre proofing
</commit_message>
<xml_diff>
--- a/text/img/speed.xlsx
+++ b/text/img/speed.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23940" windowHeight="6750" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Chart2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>NeoEloquent</t>
   </si>
@@ -43,6 +44,12 @@
   </si>
   <si>
     <t>Cypher shell</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -277,81 +284,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9B61-4735-8E86-906E298E546F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$Q$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Cypher shell</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$N$12:$N$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>200</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$Q$12:$Q$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9B61-4735-8E86-906E298E546F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -559,7 +491,444 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.0358705161854777E-2"/>
+          <c:y val="6.2465368912219307E-2"/>
+          <c:w val="0.89019685039370078"/>
+          <c:h val="0.73577136191309422"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cypher shell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$N$12:$N$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$12:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>162.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>248.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3E54-4F7B-99FF-7A7A077459E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SQL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$N$12:$N$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$12:$R$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>387.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1339.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2396.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD49-4590-B6A9-3693A36163F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="493402704"/>
+        <c:axId val="493400408"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="493402704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="493400408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="493400408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="493402704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1115,11 +1484,539 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -1131,13 +2028,46 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670192" cy="6293013"/>
+    <xdr:ext cx="8662051" cy="6293013"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0AE6755-B744-4518-BF44-AFA6C0332257}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36EAE002-7DB3-4C72-8969-9DE4DB810E3E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1457,10 +2387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="M31" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,12 +2404,12 @@
     <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1514,7 +2444,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>50</v>
       </c>
@@ -1549,7 +2479,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100</v>
       </c>
@@ -1584,12 +2514,12 @@
         <v>357</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -1628,7 +2558,7 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50</v>
       </c>
@@ -1667,7 +2597,7 @@
         <v>281.7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>100</v>
       </c>
@@ -1706,7 +2636,7 @@
         <v>705.7</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>200</v>
       </c>
@@ -1745,7 +2675,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="O11" t="s">
         <v>0</v>
       </c>
@@ -1755,8 +2685,11 @@
       <c r="Q11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -1772,11 +2705,15 @@
         <v>83.2</v>
       </c>
       <c r="Q12">
-        <f>L19</f>
+        <f>L21</f>
         <v>6.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <f t="shared" ref="R12:R18" si="1">L31</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1818,7 +2755,7 @@
         <v>50</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13" si="1">L8</f>
+        <f t="shared" ref="O13" si="2">L8</f>
         <v>281.7</v>
       </c>
       <c r="P13">
@@ -1826,11 +2763,15 @@
         <v>195</v>
       </c>
       <c r="Q13">
-        <f>L20</f>
+        <f>L22</f>
         <v>25.2</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>50</v>
       </c>
@@ -1865,7 +2806,7 @@
         <v>192</v>
       </c>
       <c r="L14">
-        <f t="shared" ref="L14" si="2">AVERAGE(B14:K14)</f>
+        <f t="shared" ref="L14" si="3">AVERAGE(B14:K14)</f>
         <v>195</v>
       </c>
       <c r="N14">
@@ -1876,15 +2817,19 @@
         <v>705.7</v>
       </c>
       <c r="P14">
-        <f t="shared" ref="P14:P15" si="3">L15</f>
+        <f t="shared" ref="P14:P15" si="4">L15</f>
         <v>358.5</v>
       </c>
       <c r="Q14">
-        <f t="shared" ref="Q14:Q15" si="4">L21</f>
+        <f t="shared" ref="Q14" si="5">L23</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>100</v>
       </c>
@@ -1930,15 +2875,18 @@
         <v>1857</v>
       </c>
       <c r="P15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>695.7</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="4"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>200</v>
       </c>
@@ -1980,311 +2928,996 @@
         <f>L16/L10</f>
         <v>0.37463651050080776</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="N16">
+        <v>500</v>
+      </c>
+      <c r="Q16">
+        <f>L25</f>
+        <v>99.8</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>387.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>1000</v>
+      </c>
+      <c r="Q17">
+        <f>L26</f>
+        <v>162.69999999999999</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>1339.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>1400</v>
+      </c>
+      <c r="Q18">
+        <f>L27</f>
+        <v>248.9</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="1"/>
+        <v>2396.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O20" t="s">
         <v>0</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P20" t="s">
         <v>3</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="Q20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>3</v>
       </c>
-      <c r="C19">
+      <c r="C21">
         <v>7</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>4</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <v>11</v>
       </c>
-      <c r="F19">
+      <c r="F21">
         <v>8</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>8</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>3</v>
       </c>
-      <c r="I19">
+      <c r="I21">
         <v>8</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>9</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>6</v>
       </c>
-      <c r="L19">
-        <f>AVERAGE(B19:K19)</f>
+      <c r="L21">
+        <f>AVERAGE(B21:K21)</f>
         <v>6.7</v>
       </c>
-      <c r="N19">
+      <c r="N21">
         <v>10</v>
       </c>
-      <c r="O19">
-        <f>O12-40</f>
+      <c r="O21">
+        <f t="shared" ref="O21:P24" si="6">O12-40</f>
         <v>61.599999999999994</v>
       </c>
-      <c r="P19">
-        <f>P12-40</f>
+      <c r="P21">
+        <f t="shared" si="6"/>
         <v>43.2</v>
       </c>
-      <c r="Q19">
+      <c r="Q21">
         <f>Q12</f>
         <v>6.7</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>50</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>20</v>
       </c>
-      <c r="C20">
+      <c r="C22">
         <v>26</v>
       </c>
-      <c r="D20">
+      <c r="D22">
         <v>24</v>
       </c>
-      <c r="E20">
+      <c r="E22">
         <v>31</v>
       </c>
-      <c r="F20">
+      <c r="F22">
         <v>31</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <v>28</v>
       </c>
-      <c r="H20">
+      <c r="H22">
         <v>26</v>
       </c>
-      <c r="I20">
+      <c r="I22">
         <v>22</v>
       </c>
-      <c r="J20">
+      <c r="J22">
         <v>22</v>
       </c>
-      <c r="K20">
+      <c r="K22">
         <v>22</v>
       </c>
-      <c r="L20">
-        <f t="shared" ref="L20:L21" si="5">AVERAGE(B20:K20)</f>
+      <c r="L22">
+        <f t="shared" ref="L22:L23" si="7">AVERAGE(B22:K22)</f>
         <v>25.2</v>
       </c>
-      <c r="N20">
+      <c r="N22">
         <v>50</v>
       </c>
-      <c r="O20">
-        <f>O13-40</f>
+      <c r="O22">
+        <f t="shared" si="6"/>
         <v>241.7</v>
       </c>
-      <c r="P20">
-        <f>P13-40</f>
+      <c r="P22">
+        <f t="shared" si="6"/>
         <v>155</v>
       </c>
-      <c r="Q20">
-        <f t="shared" ref="Q20:Q22" si="6">Q13-40</f>
+      <c r="Q22">
+        <f>Q13-40</f>
         <v>-14.8</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>100</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>39</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <v>33</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>37</v>
       </c>
-      <c r="E21">
+      <c r="E23">
         <v>35</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <v>28</v>
       </c>
-      <c r="G21">
+      <c r="G23">
         <v>30</v>
       </c>
-      <c r="H21">
+      <c r="H23">
         <v>40</v>
       </c>
-      <c r="I21">
+      <c r="I23">
         <v>28</v>
       </c>
-      <c r="J21">
+      <c r="J23">
         <v>26</v>
       </c>
-      <c r="K21">
+      <c r="K23">
         <v>24</v>
       </c>
-      <c r="L21">
-        <f t="shared" si="5"/>
+      <c r="L23">
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
-      <c r="N21">
+      <c r="N23">
         <v>100</v>
       </c>
-      <c r="O21">
-        <f>O14-40</f>
+      <c r="O23">
+        <f t="shared" si="6"/>
         <v>665.7</v>
       </c>
-      <c r="P21">
-        <f>P14-40</f>
+      <c r="P23">
+        <f t="shared" si="6"/>
         <v>318.5</v>
       </c>
-      <c r="Q21">
+      <c r="Q23">
+        <f>Q14-40</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>200</v>
+      </c>
+      <c r="B24">
+        <v>66</v>
+      </c>
+      <c r="C24">
+        <v>67</v>
+      </c>
+      <c r="D24">
+        <v>68</v>
+      </c>
+      <c r="E24">
+        <v>60</v>
+      </c>
+      <c r="F24">
+        <v>73</v>
+      </c>
+      <c r="G24">
+        <v>72</v>
+      </c>
+      <c r="H24">
+        <v>73</v>
+      </c>
+      <c r="I24">
+        <v>66</v>
+      </c>
+      <c r="J24">
+        <v>67</v>
+      </c>
+      <c r="K24">
+        <v>68</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ref="L24:L27" si="8">AVERAGE(B24:K24)</f>
+        <v>68</v>
+      </c>
+      <c r="N24">
+        <v>200</v>
+      </c>
+      <c r="O24">
         <f t="shared" si="6"/>
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22">
+        <v>1817</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="6"/>
+        <v>655.7</v>
+      </c>
+      <c r="Q24">
+        <f>Q15-40</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>500</v>
+      </c>
+      <c r="B25">
+        <v>92</v>
+      </c>
+      <c r="C25">
+        <v>99</v>
+      </c>
+      <c r="D25">
+        <v>96</v>
+      </c>
+      <c r="E25">
+        <v>97</v>
+      </c>
+      <c r="F25">
+        <v>108</v>
+      </c>
+      <c r="G25">
+        <v>96</v>
+      </c>
+      <c r="H25">
+        <v>127</v>
+      </c>
+      <c r="I25">
+        <v>97</v>
+      </c>
+      <c r="J25">
+        <v>96</v>
+      </c>
+      <c r="K25">
+        <v>90</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="8"/>
+        <v>99.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1000</v>
+      </c>
+      <c r="B26">
+        <v>163</v>
+      </c>
+      <c r="C26">
+        <v>177</v>
+      </c>
+      <c r="D26">
+        <v>154</v>
+      </c>
+      <c r="E26">
+        <v>156</v>
+      </c>
+      <c r="F26">
+        <v>153</v>
+      </c>
+      <c r="G26">
+        <v>170</v>
+      </c>
+      <c r="H26">
+        <v>151</v>
+      </c>
+      <c r="I26">
+        <v>190</v>
+      </c>
+      <c r="J26">
+        <v>164</v>
+      </c>
+      <c r="K26">
+        <v>149</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="8"/>
+        <v>162.69999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1400</v>
+      </c>
+      <c r="B27">
+        <v>277</v>
+      </c>
+      <c r="C27">
+        <v>345</v>
+      </c>
+      <c r="D27">
+        <v>254</v>
+      </c>
+      <c r="E27">
+        <v>227</v>
+      </c>
+      <c r="F27">
+        <v>218</v>
+      </c>
+      <c r="G27">
+        <v>221</v>
+      </c>
+      <c r="H27">
+        <v>226</v>
+      </c>
+      <c r="I27">
+        <v>241</v>
+      </c>
+      <c r="J27">
+        <v>241</v>
+      </c>
+      <c r="K27">
+        <v>239</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="8"/>
+        <v>248.9</v>
+      </c>
+      <c r="O27" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>4</v>
+      </c>
+      <c r="R27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>10</v>
+      </c>
+      <c r="O28" s="2">
+        <v>1</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>50</v>
+      </c>
+      <c r="O29" s="2">
+        <f t="shared" ref="O29:Q31" si="9">O13/O12</f>
+        <v>2.7726377952755907</v>
+      </c>
+      <c r="P29" s="2">
+        <f t="shared" si="9"/>
+        <v>2.34375</v>
+      </c>
+      <c r="Q29" s="2">
+        <f t="shared" si="9"/>
+        <v>3.761194029850746</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="N30">
+        <v>100</v>
+      </c>
+      <c r="O30" s="2">
+        <f t="shared" si="9"/>
+        <v>2.5051473198438057</v>
+      </c>
+      <c r="P30" s="2">
+        <f t="shared" si="9"/>
+        <v>1.8384615384615384</v>
+      </c>
+      <c r="Q30" s="2">
+        <f t="shared" si="9"/>
+        <v>1.2698412698412698</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>16</v>
+      </c>
+      <c r="E31">
+        <v>15</v>
+      </c>
+      <c r="F31">
+        <v>17</v>
+      </c>
+      <c r="G31">
+        <v>15</v>
+      </c>
+      <c r="H31">
+        <v>16</v>
+      </c>
+      <c r="I31">
+        <v>15</v>
+      </c>
+      <c r="J31">
+        <v>15</v>
+      </c>
+      <c r="K31">
+        <v>16</v>
+      </c>
+      <c r="L31">
+        <f>AVERAGE(B31:K31)</f>
+        <v>15.5</v>
+      </c>
+      <c r="N31">
         <v>200</v>
       </c>
-      <c r="B22">
-        <v>66</v>
-      </c>
-      <c r="C22">
-        <v>67</v>
-      </c>
-      <c r="D22">
-        <v>68</v>
-      </c>
-      <c r="E22">
-        <v>60</v>
-      </c>
-      <c r="F22">
-        <v>73</v>
-      </c>
-      <c r="G22">
-        <v>72</v>
-      </c>
-      <c r="H22">
-        <v>73</v>
-      </c>
-      <c r="I22">
-        <v>66</v>
-      </c>
-      <c r="J22">
-        <v>67</v>
-      </c>
-      <c r="K22">
-        <v>68</v>
-      </c>
-      <c r="L22">
-        <f t="shared" ref="L22" si="7">AVERAGE(B22:K22)</f>
-        <v>68</v>
-      </c>
-      <c r="N22">
+      <c r="O31" s="2">
+        <f t="shared" si="9"/>
+        <v>2.6314297860280571</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="9"/>
+        <v>1.9405857740585775</v>
+      </c>
+      <c r="Q31" s="2">
+        <f t="shared" si="9"/>
+        <v>1.6875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>50</v>
+      </c>
+      <c r="B32">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>17</v>
+      </c>
+      <c r="F32">
+        <v>17</v>
+      </c>
+      <c r="G32">
+        <v>15</v>
+      </c>
+      <c r="H32">
+        <v>16</v>
+      </c>
+      <c r="I32">
+        <v>16</v>
+      </c>
+      <c r="J32">
+        <v>17</v>
+      </c>
+      <c r="K32">
+        <v>16</v>
+      </c>
+      <c r="L32">
+        <f>AVERAGE(B32:K32)</f>
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>100</v>
+      </c>
+      <c r="B33">
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>32</v>
+      </c>
+      <c r="F33">
+        <v>31</v>
+      </c>
+      <c r="G33">
+        <v>35</v>
+      </c>
+      <c r="H33">
+        <v>31</v>
+      </c>
+      <c r="I33">
+        <v>32</v>
+      </c>
+      <c r="J33">
+        <v>31</v>
+      </c>
+      <c r="K33">
+        <v>30</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ref="L33:L37" si="10">AVERAGE(B33:K33)</f>
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>200</v>
       </c>
-      <c r="O22">
-        <f>O15-40</f>
-        <v>1817</v>
-      </c>
-      <c r="P22">
-        <f>P15-40</f>
-        <v>655.7</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="6"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="O25" t="s">
+      <c r="B34">
+        <v>62</v>
+      </c>
+      <c r="C34">
+        <v>62</v>
+      </c>
+      <c r="D34">
+        <v>63</v>
+      </c>
+      <c r="E34">
+        <v>62</v>
+      </c>
+      <c r="F34">
+        <v>62</v>
+      </c>
+      <c r="G34">
+        <v>62</v>
+      </c>
+      <c r="H34">
+        <v>63</v>
+      </c>
+      <c r="I34">
+        <v>64</v>
+      </c>
+      <c r="J34">
+        <v>62</v>
+      </c>
+      <c r="K34">
+        <v>63</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="10"/>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>500</v>
+      </c>
+      <c r="B35">
+        <v>390</v>
+      </c>
+      <c r="C35">
+        <v>391</v>
+      </c>
+      <c r="D35">
+        <v>390</v>
+      </c>
+      <c r="E35">
+        <v>375</v>
+      </c>
+      <c r="F35">
+        <v>390</v>
+      </c>
+      <c r="G35">
+        <v>390</v>
+      </c>
+      <c r="H35">
+        <v>391</v>
+      </c>
+      <c r="I35">
+        <v>390</v>
+      </c>
+      <c r="J35">
+        <v>391</v>
+      </c>
+      <c r="K35">
+        <v>375</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="10"/>
+        <v>387.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1000</v>
+      </c>
+      <c r="B36">
+        <v>1328</v>
+      </c>
+      <c r="C36">
+        <v>1359</v>
+      </c>
+      <c r="D36">
+        <v>1344</v>
+      </c>
+      <c r="E36">
+        <v>1321</v>
+      </c>
+      <c r="F36">
+        <v>1343</v>
+      </c>
+      <c r="G36">
+        <v>1344</v>
+      </c>
+      <c r="H36">
+        <v>1328</v>
+      </c>
+      <c r="I36">
+        <v>1343</v>
+      </c>
+      <c r="J36">
+        <v>1359</v>
+      </c>
+      <c r="K36">
+        <v>1329</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="10"/>
+        <v>1339.8</v>
+      </c>
+      <c r="O36" t="s">
+        <v>5</v>
+      </c>
+      <c r="P36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1400</v>
+      </c>
+      <c r="B37">
+        <v>2391</v>
+      </c>
+      <c r="C37">
+        <v>2391</v>
+      </c>
+      <c r="D37">
+        <v>2421</v>
+      </c>
+      <c r="E37">
+        <v>2390</v>
+      </c>
+      <c r="F37">
+        <v>2391</v>
+      </c>
+      <c r="G37">
+        <v>2375</v>
+      </c>
+      <c r="H37">
+        <v>2421</v>
+      </c>
+      <c r="I37">
+        <v>2375</v>
+      </c>
+      <c r="J37">
+        <v>2421</v>
+      </c>
+      <c r="K37">
+        <v>2390</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="10"/>
+        <v>2396.6</v>
+      </c>
+      <c r="N37">
+        <v>10</v>
+      </c>
+      <c r="O37">
+        <v>6.7</v>
+      </c>
+      <c r="P37">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>50</v>
+      </c>
+      <c r="O38">
+        <v>25.2</v>
+      </c>
+      <c r="P38">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>100</v>
+      </c>
+      <c r="O39">
+        <v>32</v>
+      </c>
+      <c r="P39">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>200</v>
+      </c>
+      <c r="O40">
+        <v>54</v>
+      </c>
+      <c r="P40">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <v>500</v>
+      </c>
+      <c r="O41">
+        <v>99.8</v>
+      </c>
+      <c r="P41">
+        <v>387.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <v>1000</v>
+      </c>
+      <c r="O42">
+        <v>162.69999999999999</v>
+      </c>
+      <c r="P42">
+        <v>1339.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N43">
+        <v>1400</v>
+      </c>
+      <c r="O43">
+        <v>248.9</v>
+      </c>
+      <c r="P43">
+        <v>2396.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <v>10</v>
+      </c>
+      <c r="P46">
+        <v>50</v>
+      </c>
+      <c r="Q46">
+        <v>100</v>
+      </c>
+      <c r="R46">
+        <v>200</v>
+      </c>
+      <c r="S46">
+        <v>500</v>
+      </c>
+      <c r="T46">
+        <v>1000</v>
+      </c>
+      <c r="U46">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>5</v>
+      </c>
+      <c r="O47">
+        <v>6.7</v>
+      </c>
+      <c r="P47">
+        <v>25.2</v>
+      </c>
+      <c r="Q47">
+        <v>32</v>
+      </c>
+      <c r="R47">
+        <v>54</v>
+      </c>
+      <c r="S47">
+        <v>99.8</v>
+      </c>
+      <c r="T47">
+        <v>162.69999999999999</v>
+      </c>
+      <c r="U47">
+        <v>248.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>6</v>
+      </c>
+      <c r="O48">
+        <v>15.5</v>
+      </c>
+      <c r="P48">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q48">
+        <v>31.6</v>
+      </c>
+      <c r="R48">
+        <v>62.5</v>
+      </c>
+      <c r="S48">
+        <v>387.3</v>
+      </c>
+      <c r="T48">
+        <v>1339.8</v>
+      </c>
+      <c r="U48">
+        <v>2396.6</v>
+      </c>
+    </row>
+    <row r="51" spans="14:18" x14ac:dyDescent="0.25">
+      <c r="O51" t="s">
         <v>0</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P51" t="s">
         <v>3</v>
       </c>
-      <c r="Q25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N26">
+    </row>
+    <row r="52" spans="14:18" x14ac:dyDescent="0.25">
+      <c r="N52">
         <v>10</v>
       </c>
-      <c r="O26" s="2">
-        <v>1</v>
-      </c>
-      <c r="P26" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N27">
+      <c r="O52">
+        <v>101.6</v>
+      </c>
+      <c r="P52">
+        <v>83.2</v>
+      </c>
+    </row>
+    <row r="53" spans="14:18" x14ac:dyDescent="0.25">
+      <c r="N53">
         <v>50</v>
       </c>
-      <c r="O27" s="2">
-        <f>O13/O12</f>
-        <v>2.7726377952755907</v>
-      </c>
-      <c r="P27" s="2">
-        <f>P13/P12</f>
-        <v>2.34375</v>
-      </c>
-      <c r="Q27" s="2">
-        <f>Q13/Q12</f>
-        <v>3.761194029850746</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N28">
+      <c r="O53">
+        <v>281.7</v>
+      </c>
+      <c r="P53">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="14:18" x14ac:dyDescent="0.25">
+      <c r="N54">
         <v>100</v>
       </c>
-      <c r="O28" s="2">
-        <f>O14/O13</f>
-        <v>2.5051473198438057</v>
-      </c>
-      <c r="P28" s="2">
-        <f>P14/P13</f>
-        <v>1.8384615384615384</v>
-      </c>
-      <c r="Q28" s="2">
-        <f>Q14/Q13</f>
-        <v>1.2698412698412698</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N29">
+      <c r="O54">
+        <v>705.7</v>
+      </c>
+      <c r="P54">
+        <v>358.5</v>
+      </c>
+    </row>
+    <row r="55" spans="14:18" x14ac:dyDescent="0.25">
+      <c r="N55">
         <v>200</v>
       </c>
-      <c r="O29" s="2">
-        <f>O15/O14</f>
-        <v>2.6314297860280571</v>
-      </c>
-      <c r="P29" s="2">
-        <f>P15/P14</f>
-        <v>1.9405857740585775</v>
-      </c>
-      <c r="Q29" s="2">
-        <f>Q15/Q14</f>
-        <v>2.125</v>
+      <c r="O55">
+        <v>1857</v>
+      </c>
+      <c r="P55">
+        <v>695.7</v>
+      </c>
+    </row>
+    <row r="57" spans="14:18" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <v>10</v>
+      </c>
+      <c r="P57">
+        <v>50</v>
+      </c>
+      <c r="Q57">
+        <v>100</v>
+      </c>
+      <c r="R57">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="14:18" x14ac:dyDescent="0.25">
+      <c r="N58" t="s">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>101.6</v>
+      </c>
+      <c r="P58">
+        <v>281.7</v>
+      </c>
+      <c r="Q58">
+        <v>705.7</v>
+      </c>
+      <c r="R58">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="59" spans="14:18" x14ac:dyDescent="0.25">
+      <c r="N59" t="s">
+        <v>3</v>
+      </c>
+      <c r="O59">
+        <v>83.2</v>
+      </c>
+      <c r="P59">
+        <v>195</v>
+      </c>
+      <c r="Q59">
+        <v>358.5</v>
+      </c>
+      <c r="R59">
+        <v>695.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>